<commit_message>
Add task expulsion table
</commit_message>
<xml_diff>
--- a/time_analisys.xlsx
+++ b/time_analisys.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27103"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0736BBB4-4513-40D8-AAD0-8BF508A0BE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{099CAAC4-7BF4-4039-A4B2-393E69EB6FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
   <si>
     <t>Cabeza</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Deadline (ms):</t>
+  </si>
+  <si>
+    <t>Expulsiones</t>
   </si>
   <si>
     <t>Inicio Esperado (ms)</t>
@@ -60,13 +63,25 @@
     <t>Restante (ms)</t>
   </si>
   <si>
-    <t>Distancia</t>
+    <t>Proceso Expulsado</t>
+  </si>
+  <si>
+    <t>Proceso Expulsor</t>
+  </si>
+  <si>
+    <t>Instante Expulsado (ms)</t>
+  </si>
+  <si>
+    <t>Display (10)</t>
+  </si>
+  <si>
+    <t>Riesgos</t>
   </si>
   <si>
     <t>Volante</t>
   </si>
   <si>
-    <t>Riesgos</t>
+    <t>Distancia</t>
   </si>
   <si>
     <t>Display</t>
@@ -114,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -279,11 +294,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -298,6 +322,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,6 +393,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -395,6 +443,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -420,36 +478,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -916,9 +944,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:H51"/>
+  <dimension ref="B2:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -927,10 +955,12 @@
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
-    <col min="6" max="14" width="18.85546875" customWidth="1"/>
+    <col min="6" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="12" width="25.140625" customWidth="1"/>
+    <col min="13" max="14" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:12">
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
@@ -949,28 +979,42 @@
       <c r="H2" s="13">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="3" spans="2:8">
+      <c r="J2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="15"/>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3" spans="2:12">
       <c r="B3" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8">
+        <v>9</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
       <c r="B4" s="1">
         <v>0</v>
       </c>
@@ -992,8 +1036,17 @@
         <f>F4-G4</f>
         <v>6.5856600000000015E-2</v>
       </c>
-    </row>
-    <row r="5" spans="2:8">
+      <c r="J4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.15091979999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
       <c r="B5" s="1">
         <f>B4+D$2</f>
         <v>0.4</v>
@@ -1016,8 +1069,17 @@
         <f t="shared" ref="H5:H9" si="2">F5-G5</f>
         <v>8.3203199999999977E-2</v>
       </c>
-    </row>
-    <row r="6" spans="2:8">
+      <c r="J5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1.0508305</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
       <c r="B6" s="1">
         <f t="shared" ref="B6:B9" si="3">B5+D$2</f>
         <v>0.8</v>
@@ -1040,8 +1102,17 @@
         <f t="shared" si="2"/>
         <v>8.3200700000000016E-2</v>
       </c>
-    </row>
-    <row r="7" spans="2:8">
+      <c r="J6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1.0784786</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7" s="1">
         <f t="shared" si="3"/>
         <v>1.2000000000000002</v>
@@ -1065,7 +1136,7 @@
         <v>8.3179100000000172E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:12">
       <c r="B8" s="1">
         <f t="shared" si="3"/>
         <v>1.6</v>
@@ -1089,7 +1160,7 @@
         <v>8.3200100000000221E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:12">
       <c r="B9" s="2">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -1113,9 +1184,9 @@
         <v>8.3192600000000283E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:12">
       <c r="B11" s="10" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>1</v>
@@ -1124,7 +1195,7 @@
         <v>0.3</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>2</v>
@@ -1133,27 +1204,27 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:12">
       <c r="B12" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
       <c r="B13" s="1">
         <v>0</v>
       </c>
@@ -1176,7 +1247,7 @@
         <v>0.20218589999999997</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:12">
       <c r="B14" s="1">
         <f>B13+D$11</f>
         <v>0.3</v>
@@ -1200,7 +1271,7 @@
         <v>0.2490405</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:12">
       <c r="B15" s="1">
         <f>B14+D$11</f>
         <v>0.6</v>
@@ -1224,7 +1295,7 @@
         <v>0.24924989999999991</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:12">
       <c r="B16" s="1">
         <f>B15+D$11</f>
         <v>0.89999999999999991</v>
@@ -1322,7 +1393,7 @@
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>1</v>
@@ -1331,7 +1402,7 @@
         <v>0.35</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>2</v>
@@ -1342,22 +1413,22 @@
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -1505,7 +1576,7 @@
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>1</v>
@@ -1514,7 +1585,7 @@
         <v>0.15</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G30" s="11" t="s">
         <v>2</v>
@@ -1525,22 +1596,22 @@
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="2:8">
@@ -1880,7 +1951,7 @@
     </row>
     <row r="47" spans="2:8">
       <c r="B47" s="10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>1</v>
@@ -1889,7 +1960,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G47" s="11" t="s">
         <v>2</v>
@@ -1900,22 +1971,22 @@
     </row>
     <row r="48" spans="2:8">
       <c r="B48" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="2:8">
@@ -1967,7 +2038,7 @@
     </row>
     <row r="51" spans="2:8">
       <c r="B51" s="2">
-        <f t="shared" ref="B51:B62" si="10">B50+D$47</f>
+        <f t="shared" ref="B51" si="10">B50+D$47</f>
         <v>2</v>
       </c>
       <c r="C51" s="5">
@@ -1991,116 +2062,116 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4:H9">
-    <cfRule type="cellIs" dxfId="29" priority="43" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="29" priority="46" operator="greaterThanOrEqual">
       <formula xml:space="preserve"> 2 * $H$2 / 3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="44" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="47" operator="greaterThanOrEqual">
       <formula xml:space="preserve"> 1 * $H$2 / 3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="45" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="27" priority="48" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H19">
-    <cfRule type="cellIs" dxfId="26" priority="42" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="45" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H19">
-    <cfRule type="cellIs" dxfId="25" priority="36" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="39" operator="greaterThanOrEqual">
       <formula xml:space="preserve"> 2 * $H$11 / 4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H19">
-    <cfRule type="cellIs" dxfId="24" priority="38" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="41" operator="greaterThanOrEqual">
       <formula xml:space="preserve"> 1 * $H$11 / 4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23:H28">
-    <cfRule type="cellIs" dxfId="23" priority="32" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="23" priority="35" operator="greaterThanOrEqual">
       <formula xml:space="preserve"> 2*$H$21 / 3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="33" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="36" operator="greaterThanOrEqual">
       <formula xml:space="preserve"> 1*$H$21 / 3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="34" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="21" priority="37" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H45">
-    <cfRule type="cellIs" dxfId="20" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="30" operator="greaterThanOrEqual">
       <formula xml:space="preserve"> 2*$H$30 / 3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="28" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="19" priority="31" operator="greaterThanOrEqual">
       <formula xml:space="preserve"> 1*$H$30 / 3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="29" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="32" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D9">
-    <cfRule type="cellIs" dxfId="17" priority="22" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="25" operator="lessThanOrEqual">
       <formula>1*$H$2 / 3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="23" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="26" operator="lessThanOrEqual">
       <formula>2*$H$2 / 3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="27" operator="lessThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:D19">
-    <cfRule type="cellIs" dxfId="14" priority="20" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="lessThanOrEqual">
+      <formula>$H$11/3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="23" operator="lessThanOrEqual">
       <formula>2*$H$11/3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="lessThanOrEqual">
-      <formula>$H$11/3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="21" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="24" operator="lessThanOrEqual">
       <formula>$H$11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D28">
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="lessThanOrEqual">
       <formula>$H$21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="lessThanOrEqual">
       <formula>2*$H$21/3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="20" operator="lessThanOrEqual">
       <formula>$H$21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D45">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="lessThanOrEqual">
+      <formula>1*$H$30/3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="lessThanOrEqual">
       <formula>2*$H$30/3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="lessThanOrEqual">
       <formula>$H$30</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThanOrEqual">
-      <formula>1*$H$30/3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49:H51">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThanOrEqual">
       <formula xml:space="preserve"> 2*$H$47 / 3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThanOrEqual">
       <formula xml:space="preserve"> 1*$H$47 / 3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:D51">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThanOrEqual">
       <formula>1*$H$47/3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThanOrEqual">
       <formula>2*$H$47/3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThanOrEqual">
       <formula>$H$47</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>